<commit_message>
Erste Haelfte Staffel 6 Normalos
</commit_message>
<xml_diff>
--- a/data/normalo2025.xlsx
+++ b/data/normalo2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelhaas/Documents/Coding/aytogermany/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80C608F-C557-054A-ACC5-F441B6297C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F089CA-B26E-B745-9889-42750159F45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8920" yWindow="780" windowWidth="25000" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12320" yWindow="780" windowWidth="21880" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nights" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
   <si>
     <t>Lights</t>
   </si>
@@ -54,6 +54,39 @@
   </si>
   <si>
     <t>Sinan</t>
+  </si>
+  <si>
+    <t>Deisy</t>
+  </si>
+  <si>
+    <t>Ina</t>
+  </si>
+  <si>
+    <t>Joanna</t>
+  </si>
+  <si>
+    <t>Tori</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>Selina</t>
+  </si>
+  <si>
+    <t>Camelia</t>
+  </si>
+  <si>
+    <t>Nadja</t>
+  </si>
+  <si>
+    <t>Chiara</t>
+  </si>
+  <si>
+    <t>Nasti</t>
   </si>
 </sst>
 </file>
@@ -81,12 +114,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -116,13 +161,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,15 +471,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="B1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -468,145 +514,180 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
cleanup/refactoring, Daten Doppelfolge 6
</commit_message>
<xml_diff>
--- a/data/normalo2025.xlsx
+++ b/data/normalo2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelhaas/Documents/Coding/aytogermany/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F089CA-B26E-B745-9889-42750159F45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872C344B-6A0F-ED46-83E6-5E8C5A282C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12320" yWindow="780" windowWidth="21880" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14760" yWindow="780" windowWidth="19440" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nights" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="22">
   <si>
     <t>Lights</t>
   </si>
@@ -114,7 +114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +130,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,14 +173,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L6"/>
+  <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -515,19 +530,19 @@
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G2" t="s">
@@ -542,7 +557,7 @@
       <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L2">
@@ -550,22 +565,22 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H3" t="s">
@@ -577,7 +592,7 @@
       <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L3">
@@ -585,34 +600,34 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L4">
@@ -620,34 +635,34 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L5">
@@ -655,38 +670,73 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L6">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>